<commit_message>
update instruction set - add beqz
</commit_message>
<xml_diff>
--- a/documents/IAM-INSTRUCTION-SET.xlsx
+++ b/documents/IAM-INSTRUCTION-SET.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="IAM-IS" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="128">
   <si>
     <t>R-type</t>
   </si>
@@ -232,7 +232,7 @@
     <t>beq</t>
   </si>
   <si>
-    <t>rt == rt, PC = PC + 4 + addr * 4</t>
+    <t>rt == rt, PC = PC + addr * 4</t>
   </si>
   <si>
     <t>Byte</t>
@@ -244,7 +244,19 @@
     <t>bneq</t>
   </si>
   <si>
-    <t>rt != rt, PC = PC + 4 + addr * 4</t>
+    <t>rt != rt, PC = PC + addr * 4</t>
+  </si>
+  <si>
+    <t>Branch Equal to Zero</t>
+  </si>
+  <si>
+    <t>beqz</t>
+  </si>
+  <si>
+    <t>rt == 0, PC = PC + addr * 4</t>
+  </si>
+  <si>
+    <t>Offset</t>
   </si>
   <si>
     <t>Branch &lt; 0</t>
@@ -253,10 +265,7 @@
     <t>bltz</t>
   </si>
   <si>
-    <t>rt &lt; 0, PC = PC + 4 + addr * 4</t>
-  </si>
-  <si>
-    <t>Offset</t>
+    <t>rt &lt; 0, PC = PC + addr * 4</t>
   </si>
   <si>
     <t>Branch &gt; 0</t>
@@ -265,7 +274,16 @@
     <t>bgtz</t>
   </si>
   <si>
-    <t>rt &gt; 0, PC = PC + 4 + addr * 4</t>
+    <t>rt &gt; 0, PC = PC + addr * 4</t>
+  </si>
+  <si>
+    <t>Registers</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Use</t>
   </si>
   <si>
     <t>Branch &lt;</t>
@@ -274,16 +292,7 @@
     <t>blt</t>
   </si>
   <si>
-    <t>rt &lt; rs, PC = PC + 4 + addr * 4</t>
-  </si>
-  <si>
-    <t>Registers</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Use</t>
+    <t>rt &lt; rs, PC = PC + addr * 4</t>
   </si>
   <si>
     <t>Branch &gt;</t>
@@ -292,7 +301,13 @@
     <t>bgt</t>
   </si>
   <si>
-    <t>rt &gt; rs, PC = PC + 4 + addr * 4</t>
+    <t>rt &gt; rs, PC = PC + addr * 4</t>
+  </si>
+  <si>
+    <t>$zero</t>
+  </si>
+  <si>
+    <t>Constant 0 value</t>
   </si>
   <si>
     <t>Load Word</t>
@@ -304,12 +319,6 @@
     <t>rt = M[rs + imm]</t>
   </si>
   <si>
-    <t>$zero</t>
-  </si>
-  <si>
-    <t>Constant 0 value</t>
-  </si>
-  <si>
     <t>Store Word</t>
   </si>
   <si>
@@ -319,6 +328,15 @@
     <t>M[rs + imm] = rt</t>
   </si>
   <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>$r0-$r28</t>
+  </si>
+  <si>
+    <t>General Purpose Registers</t>
+  </si>
+  <si>
     <t>Load Half Word</t>
   </si>
   <si>
@@ -328,13 +346,7 @@
     <t>rt = M[{rs + imm}(15:0|31:16)]</t>
   </si>
   <si>
-    <t>0x0A</t>
-  </si>
-  <si>
-    <t>$r0-$r28</t>
-  </si>
-  <si>
-    <t>General Purpose Registers</t>
+    <t>0x0B</t>
   </si>
   <si>
     <t>Store Half Word</t>
@@ -346,7 +358,7 @@
     <t>M[{rs + imm}(15:0|31:16)] = rt</t>
   </si>
   <si>
-    <t>0x0B</t>
+    <t>0x0C</t>
   </si>
   <si>
     <t>$sp</t>
@@ -373,6 +385,9 @@
     <t>PC = addr</t>
   </si>
   <si>
+    <t>Registers are 32 bit, addressible mem range is 64KB (16 bit)</t>
+  </si>
+  <si>
     <t>Jump and Link</t>
   </si>
   <si>
@@ -380,16 +395,13 @@
   </si>
   <si>
     <t>$sp = addr; PC = addr</t>
-  </si>
-  <si>
-    <t>Registers are 32 bit, addressible mem range is 64KB (16 bit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -413,6 +425,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -543,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -610,14 +627,29 @@
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" textRotation="255" vertical="center"/>
@@ -646,7 +678,7 @@
     <xf borderId="4" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1279,36 +1311,36 @@
       <c r="C17" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="29" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="3"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="L17" s="29" t="s">
+      <c r="L17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="P17" s="29" t="s">
+      <c r="P17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="Q17" s="29" t="s">
+      <c r="Q17" s="30" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1319,7 +1351,7 @@
       <c r="C18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="31" t="s">
         <v>77</v>
       </c>
       <c r="E18" s="27" t="s">
@@ -1337,20 +1369,20 @@
       <c r="Q18" s="10"/>
     </row>
     <row r="19">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="33" t="s">
         <v>38</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="34" t="s">
         <v>81</v>
       </c>
       <c r="J19" s="6">
@@ -1385,54 +1417,54 @@
       <c r="C20" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="35" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="B21" s="14" t="s">
+    <row r="21">
+      <c r="B21" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="33" t="s">
         <v>48</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="36" t="s">
         <v>88</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="32" t="s">
+      <c r="K21" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="33" t="s">
+      <c r="L21" s="38" t="s">
         <v>90</v>
       </c>
       <c r="M21" s="20"/>
       <c r="N21" s="21"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" ht="14.25" customHeight="1">
       <c r="B22" s="12" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="35" t="s">
         <v>54</v>
       </c>
       <c r="F22" s="3"/>
@@ -1444,27 +1476,27 @@
       <c r="N22" s="24"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="33" t="s">
         <v>58</v>
       </c>
       <c r="F23" s="3"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="34" t="s">
+      <c r="J23" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="40">
         <v>0.0</v>
       </c>
-      <c r="L23" s="36" t="s">
+      <c r="L23" s="41" t="s">
         <v>98</v>
       </c>
       <c r="M23" s="20"/>
@@ -1477,10 +1509,10 @@
       <c r="C24" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="35" t="s">
         <v>64</v>
       </c>
       <c r="F24" s="3"/>
@@ -1492,27 +1524,27 @@
       <c r="N24" s="24"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="33" t="s">
         <v>105</v>
       </c>
       <c r="F25" s="3"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="K25" s="37">
+      <c r="K25" s="42">
         <v>0.06180555555555556</v>
       </c>
-      <c r="L25" s="38" t="s">
+      <c r="L25" s="43" t="s">
         <v>107</v>
       </c>
       <c r="M25" s="20"/>
@@ -1525,10 +1557,10 @@
       <c r="C26" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="35" t="s">
         <v>111</v>
       </c>
       <c r="F26" s="3"/>
@@ -1540,27 +1572,33 @@
       <c r="N26" s="24"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
+      <c r="B27" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="3"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="K27" s="35">
+      <c r="J27" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" s="40">
         <v>30.0</v>
       </c>
-      <c r="L27" s="36" t="s">
-        <v>113</v>
+      <c r="L27" s="41" t="s">
+        <v>117</v>
       </c>
       <c r="M27" s="20"/>
       <c r="N27" s="21"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
       <c r="I28" s="9"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -1569,44 +1607,38 @@
       <c r="N28" s="24"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>3</v>
-      </c>
+      <c r="B29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="3"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="K29" s="39">
+      <c r="J29" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="K29" s="44">
         <v>31.0</v>
       </c>
-      <c r="L29" s="38" t="s">
-        <v>116</v>
+      <c r="L29" s="43" t="s">
+        <v>120</v>
       </c>
       <c r="M29" s="20"/>
       <c r="N29" s="21"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>105</v>
+      <c r="B30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>3</v>
       </c>
       <c r="F30" s="3"/>
       <c r="I30" s="10"/>
@@ -1617,21 +1649,21 @@
       <c r="N30" s="24"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="15" t="s">
+      <c r="B31" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="C31" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="28" t="s">
-        <v>111</v>
+      <c r="D31" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>105</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="I31" s="40" t="s">
-        <v>123</v>
+      <c r="I31" s="45" t="s">
+        <v>124</v>
       </c>
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
@@ -1640,6 +1672,19 @@
       <c r="N31" s="21"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
+      <c r="B32" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="3"/>
       <c r="I32" s="22"/>
       <c r="J32" s="23"/>
       <c r="K32" s="23"/>
@@ -2615,43 +2660,34 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
+  <mergeCells count="60">
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="M17:M18"/>
     <mergeCell ref="L21:N22"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="L23:N24"/>
+    <mergeCell ref="L25:N26"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="L25:N26"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="J15:K16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="I21:I30"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:N28"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="L29:N30"/>
-    <mergeCell ref="I31:N32"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="I2:I9"/>
     <mergeCell ref="J2:J3"/>
@@ -2667,15 +2703,26 @@
     <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="L8:P8"/>
     <mergeCell ref="L9:P9"/>
-    <mergeCell ref="I11:I18"/>
-    <mergeCell ref="J11:Q12"/>
     <mergeCell ref="J13:M14"/>
     <mergeCell ref="N13:Q14"/>
     <mergeCell ref="P15:Q16"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J11:Q12"/>
+    <mergeCell ref="I11:I18"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="I21:I30"/>
+    <mergeCell ref="L29:N30"/>
+    <mergeCell ref="I31:N32"/>
+    <mergeCell ref="B29:F29"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:N28"/>
+    <mergeCell ref="J15:K16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>